<commit_message>
Correlating Articles with Books
</commit_message>
<xml_diff>
--- a/ResearchDevelopment/Correlation4Versioning.xlsx
+++ b/ResearchDevelopment/Correlation4Versioning.xlsx
@@ -290,9 +290,6 @@
     <t>BarkleyS17</t>
   </si>
   <si>
-    <t>1888-08-12 (Butcher Shops and Canned Meat Factories)</t>
-  </si>
-  <si>
     <t>WSGC19</t>
   </si>
   <si>
@@ -321,6 +318,9 @@
   </si>
   <si>
     <t>BarkleyS23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Butcher Shops and Canned Meat Factories) 1888-08-12 </t>
   </si>
 </sst>
 </file>
@@ -362,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,6 +373,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,13 +660,13 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="61" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" style="2" customWidth="1"/>
@@ -685,7 +688,7 @@
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -699,7 +702,7 @@
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -707,7 +710,7 @@
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -715,7 +718,7 @@
       <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -729,7 +732,7 @@
       <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -743,7 +746,7 @@
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -757,7 +760,7 @@
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -771,7 +774,7 @@
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -779,7 +782,7 @@
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -793,7 +796,7 @@
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -807,7 +810,7 @@
       <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -821,7 +824,7 @@
       <c r="A13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -835,7 +838,7 @@
       <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -849,8 +852,8 @@
       <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>88</v>
+      <c r="B15" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>86</v>
@@ -863,7 +866,7 @@
       <c r="A16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -871,35 +874,35 @@
       <c r="A17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -907,49 +910,49 @@
       <c r="A20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -957,7 +960,7 @@
       <c r="A24" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -965,7 +968,7 @@
       <c r="A25" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -973,7 +976,7 @@
       <c r="A26" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -981,7 +984,7 @@
       <c r="A27" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -989,7 +992,7 @@
       <c r="A28" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -997,7 +1000,7 @@
       <c r="A29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1005,7 +1008,7 @@
       <c r="A30" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1013,7 +1016,7 @@
       <c r="A31" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1021,7 +1024,7 @@
       <c r="A32" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1029,7 +1032,7 @@
       <c r="A33" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="5" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edit to the Excel Correlation File and Creation of the Site Index
the information in the old Excel Correlation4Versioning file have been
incorporated into the Site Index and the Site Index list are complete we
just need to add the McEnnis Source into a listBibl and add notes to the
the listNym
</commit_message>
<xml_diff>
--- a/ResearchDevelopment/Correlation4Versioning.xlsx
+++ b/ResearchDevelopment/Correlation4Versioning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Becca\Documents\GitHub\CitySlaveGirls-ChicagoDailyTimes1888\researchDevelopment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Becca\Documents\GitHub\CitySlaveGirls-ChicagoDailyTimes1888\ResearchDevelopment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -317,9 +317,6 @@
     <t xml:space="preserve">(Butcher Shops and Canned Meat Factories) 1888-08-12 </t>
   </si>
   <si>
-    <t>WSGC01 WSGC02 WSGC02</t>
-  </si>
-  <si>
     <t>BarkleyS01 BarkleyS02 and BarkleyS03</t>
   </si>
   <si>
@@ -327,6 +324,9 @@
   </si>
   <si>
     <t>WSGC04 WSGC05</t>
+  </si>
+  <si>
+    <t>WSGC01 WSGC02 WSGC03</t>
   </si>
 </sst>
 </file>
@@ -663,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,10 +698,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -712,10 +712,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -997,7 +997,7 @@
         <v>59</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1005,7 +1005,7 @@
         <v>60</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1013,7 +1013,7 @@
         <v>61</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
         <v>62</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1029,7 +1029,7 @@
         <v>63</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1037,7 +1037,7 @@
         <v>64</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1045,14 +1045,14 @@
         <v>65</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>